<commit_message>
TFinal - Draft modelo de dados
ver script SQL e notas em Tarefas.xlsx
</commit_message>
<xml_diff>
--- a/TrabalhoFinal/Tarefas.xlsx
+++ b/TrabalhoFinal/Tarefas.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederico\Dropbox\ISEL\ASI\Projecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederico\work\ISEL\github\com.isel.si1314.asi\TrabalhoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12300"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12300" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tarefas" sheetId="1" r:id="rId1"/>
     <sheet name="Glossário" sheetId="4" r:id="rId2"/>
+    <sheet name="Notas do Desenvolvimento" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="132">
   <si>
     <t xml:space="preserve">Termo </t>
   </si>
@@ -308,6 +309,134 @@
   </si>
   <si>
     <t>Multi-loja</t>
+  </si>
+  <si>
+    <t>» Assumindo que vamos usar queues de mensagens entre os locais de vendas e a sede, não é preciso ter nos locais mais que (parte) da tabela de produtos. Mas achamos que deverá manter a designação e o preço, para além dos campos referidos no enunciado: Codigo e quantidade em stock</t>
+  </si>
+  <si>
+    <t>» Falta: concluir o script para ligar às diferentes bases de dados</t>
+  </si>
+  <si>
+    <t>» Na sede deverá ser necessario ter o preço do produto (mas também pode vir na venda), para as previsiveis actividades de gestao.</t>
+  </si>
+  <si>
+    <t>Modulos a Implementar</t>
+  </si>
+  <si>
+    <t>» São registados os dados do cliente: Nome e Morada (NIF?, Ntelefone?)</t>
+  </si>
+  <si>
+    <t>» Os items serão introduzidos por consulta a uma lista de produtos</t>
+  </si>
+  <si>
+    <t>» Introduzida a quantidade é calculado o preço total do item e da Venda</t>
+  </si>
+  <si>
+    <t>» No fecho inica uma transação para enviar a Venda para a "FilaVendas"  e decrementa o stock de cada produto vendido. Em caso de erro volta ao ecran de registo da venda comunicando o resultado.</t>
+  </si>
+  <si>
+    <t>VENDA - LOJA</t>
+  </si>
+  <si>
+    <t>VENDA - SEDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">» para cada VENDA recebida consulta o stock e se não tiver lança uma encomenda pela </t>
+  </si>
+  <si>
+    <t>? A ponderar: Se o stock não for suficiente lança encomenda da diferença? E se outros processos tiverem a mesma necessidade? Criar uma alternativa "quantidades Cativas?"</t>
+  </si>
+  <si>
+    <t>» Marca o item e a Venda como estando à espera da chegada de uma Encomenda"</t>
+  </si>
+  <si>
+    <t>ENCOMENDAS</t>
+  </si>
+  <si>
+    <t>» processo na sede</t>
+  </si>
+  <si>
+    <t>» As encomendas são colocadas na sequencia de uma VENDA, quando desce abaixo da quantidade minima</t>
+  </si>
+  <si>
+    <t>» Recpeção da Encomenda, actualiza stocks na SEDE e na LOJA</t>
+  </si>
+  <si>
+    <t>» como notificar a "Expedição " que pode expedir mais uma venda ?</t>
+  </si>
+  <si>
+    <t>EXPEDIÇÂO</t>
+  </si>
+  <si>
+    <t>» para todas as VENDAS em condiçoes de expedição (com qtd suficientes em stock) dentro de uma transação cria registo em Expedição e fecha a VENDA</t>
+  </si>
+  <si>
+    <t>gstFORNECEDORES</t>
+  </si>
+  <si>
+    <t>» sede</t>
+  </si>
+  <si>
+    <t>» cria e altera fornecedores</t>
+  </si>
+  <si>
+    <t>gstPRODUTOS</t>
+  </si>
+  <si>
+    <t>» Sede e Loja</t>
+  </si>
+  <si>
+    <t>» em transação sincrona, cria um produto na sede e propaga para a Loja respectiva.</t>
+  </si>
+  <si>
+    <t>» mais ou menos Comum com a alteraçao de Stocks</t>
+  </si>
+  <si>
+    <t>LISTAGEM</t>
+  </si>
+  <si>
+    <t>» apenas na SEDE</t>
+  </si>
+  <si>
+    <t>» Fornecedores, Produtos, Vendas, Expedições</t>
+  </si>
+  <si>
+    <t>» Uma vez que cada Loja controla os seus Stocks de venda, poderá não vender quando a quantidade em Stock for igual a zero, logo na sede há sempre produtos e as encomendas são para repor minimos. Ver como colocar isto a simplificar o código.</t>
+  </si>
+  <si>
+    <t>FilaVenda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">» esta fila tem uma mensagem por cada encomenda </t>
+  </si>
+  <si>
+    <t>» a estrutura deverá ter a informação necessária para colocar na tabela VENDA e VENDAPRODUTO</t>
+  </si>
+  <si>
+    <t>» Dependendo da forma como recebe a mensagem poderá ou não ser sessionless e é melhor se for (ou seja toda a info numa única mensagem);</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOTA: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tem de haver uma fila em cada servidor de Loja LHD e LSC e invocam um serviço no Servidor da SEDE (na retirada da mensgem da Queue).</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -379,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -401,6 +530,9 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,7 +840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
@@ -1034,7 +1166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="D42" sqref="D1:G1048576"/>
     </sheetView>
   </sheetViews>
@@ -1201,4 +1333,209 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:B51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="80.5703125" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>